<commit_message>
Separate tasks for customer DAG
</commit_message>
<xml_diff>
--- a/dags/customers.xlsx
+++ b/dags/customers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\bijikuda\learn-de\airflow\dags\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EC1D5C-66B7-48C8-8451-A2762F57BA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13F8D88-0226-4B2F-835D-096921CB7CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -145,10 +145,10 @@
     <t>2024-03-18 08:00:00 +0700</t>
   </si>
   <si>
+    <t>Customer 2</t>
+  </si>
+  <si>
     <t>Customer 1</t>
-  </si>
-  <si>
-    <t>Customer 2</t>
   </si>
 </sst>
 </file>
@@ -519,13 +519,13 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -549,7 +549,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -563,7 +563,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Add DAG for fact and mart daily
</commit_message>
<xml_diff>
--- a/dags/customers.xlsx
+++ b/dags/customers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\bijikuda\learn-de\airflow\dags\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6BC5F97-6B41-473A-9516-DED81887363D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30EC920-456E-4598-90EB-A3CF4581A539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>customer_id</t>
   </si>
@@ -34,121 +34,28 @@
     <t>registration_date</t>
   </si>
   <si>
-    <t>CUST0002</t>
-  </si>
-  <si>
-    <t>CUST0003</t>
-  </si>
-  <si>
-    <t>CUST0004</t>
-  </si>
-  <si>
-    <t>CUST0005</t>
-  </si>
-  <si>
-    <t>CUST0006</t>
-  </si>
-  <si>
-    <t>CUST0007</t>
-  </si>
-  <si>
-    <t>CUST0008</t>
-  </si>
-  <si>
-    <t>CUST0009</t>
-  </si>
-  <si>
-    <t>CUST0010</t>
-  </si>
-  <si>
-    <t>Customer 3</t>
-  </si>
-  <si>
-    <t>Customer 4</t>
-  </si>
-  <si>
-    <t>Customer 5</t>
-  </si>
-  <si>
-    <t>Customer 6</t>
-  </si>
-  <si>
-    <t>Customer 7</t>
-  </si>
-  <si>
-    <t>Customer 8</t>
-  </si>
-  <si>
-    <t>Customer 9</t>
-  </si>
-  <si>
-    <t>Customer 10</t>
-  </si>
-  <si>
-    <t>customer1@example.com</t>
-  </si>
-  <si>
-    <t>customer2@example.com</t>
-  </si>
-  <si>
-    <t>customer3@example.com</t>
-  </si>
-  <si>
-    <t>customer4@example.com</t>
-  </si>
-  <si>
-    <t>customer5@example.com</t>
-  </si>
-  <si>
-    <t>customer6@example.com</t>
-  </si>
-  <si>
-    <t>customer7@example.com</t>
-  </si>
-  <si>
-    <t>customer8@example.com</t>
-  </si>
-  <si>
-    <t>customer9@example.com</t>
-  </si>
-  <si>
-    <t>customer10@example.com</t>
-  </si>
-  <si>
     <t>2024-02-07 08:00:00 +0700</t>
   </si>
   <si>
     <t>2023-12-26 08:00:00 +0700</t>
   </si>
   <si>
-    <t>2024-12-07 08:00:00 +0700</t>
-  </si>
-  <si>
-    <t>2024-12-17 08:00:00 +0700</t>
-  </si>
-  <si>
-    <t>2024-05-02 08:00:00 +0700</t>
-  </si>
-  <si>
-    <t>2024-09-11 08:00:00 +0700</t>
-  </si>
-  <si>
-    <t>2024-08-23 08:00:00 +0700</t>
-  </si>
-  <si>
-    <t>2024-10-28 08:00:00 +0700</t>
-  </si>
-  <si>
-    <t>2024-03-18 08:00:00 +0700</t>
-  </si>
-  <si>
-    <t>Customer 2</t>
-  </si>
-  <si>
-    <t>Customer 1</t>
-  </si>
-  <si>
-    <t>CUST0001</t>
+    <t>cust_1</t>
+  </si>
+  <si>
+    <t>Pororo</t>
+  </si>
+  <si>
+    <t>pororo@gmail.com</t>
+  </si>
+  <si>
+    <t>Crong</t>
+  </si>
+  <si>
+    <t>crong@gmail.com</t>
+  </si>
+  <si>
+    <t>cust_2</t>
   </si>
 </sst>
 </file>
@@ -516,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,142 +453,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>